<commit_message>
OSU PSI done and uploaded
</commit_message>
<xml_diff>
--- a/data/MANUAL_Nov_2_MSU_GAME_SCORES.xlsx
+++ b/data/MANUAL_Nov_2_MSU_GAME_SCORES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\college_hockey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C7D318-B655-491A-A301-4B4B765DCFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5289F748-D915-47D7-A209-EF70A4DF6FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-16050" yWindow="4545" windowWidth="18900" windowHeight="11505" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nov_2_MSU_GAME_SCORES" sheetId="1" r:id="rId1"/>
@@ -818,7 +818,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -827,7 +827,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -844,9 +843,6 @@
     <xf numFmtId="0" fontId="22" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="23" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -858,25 +854,30 @@
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="164" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -923,17 +924,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -970,206 +961,6 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="164" formatCode="0.000"/>
       <fill>
         <patternFill patternType="solid">
@@ -1178,30 +969,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1240,28 +1007,28 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1290,28 +1057,28 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1340,28 +1107,28 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1390,6 +1157,31 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1415,6 +1207,31 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1425,6 +1242,180 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1466,6 +1457,19 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
         <name val="Roboto Slab"/>
@@ -1477,19 +1481,6 @@
           <bgColor rgb="FF18453B"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1741,7 +1732,7 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="CAN_2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="BC_1"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BC_2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="SEASON_AVG" dataDxfId="26">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="SEASON_AVG" dataDxfId="25">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[LSSU_1]:[BC_2]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1750,7 +1741,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD3ED04E-82AE-4CFB-A8EC-BB33F4837DB9}" name="Table14" displayName="Table14" ref="A5:J31" totalsRowCount="1" headerRowDxfId="24" dataDxfId="25" totalsRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD3ED04E-82AE-4CFB-A8EC-BB33F4837DB9}" name="Table14" displayName="Table14" ref="A5:J31" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22">
   <autoFilter ref="A5:J30" xr:uid="{FD3ED04E-82AE-4CFB-A8EC-BB33F4837DB9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1767,32 +1758,32 @@
     <sortCondition descending="1" ref="J5:J29"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{92A4CFC6-961E-4C81-A091-04B59744BA36}" name="Player" totalsRowLabel="TOTAL" dataDxfId="22" totalsRowDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{018653C9-4BD5-4955-BD88-FF0901ED735D}" name="LSSU_1" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{92A4CFC6-961E-4C81-A091-04B59744BA36}" name="Player" totalsRowLabel="TOTAL" dataDxfId="21" totalsRowDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{018653C9-4BD5-4955-BD88-FF0901ED735D}" name="LSSU_1" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
       <totalsRowFormula>SUM(B6:B29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8AA04EE0-25FB-4161-8387-A764CBF8C414}" name="LSSU_2" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="9">
+    <tableColumn id="3" xr3:uid="{8AA04EE0-25FB-4161-8387-A764CBF8C414}" name="LSSU_2" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
       <totalsRowFormula>SUM(C6:C29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{85A196E6-04A4-435C-9244-08FABA40BC61}" name="AF_1" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="8">
+    <tableColumn id="4" xr3:uid="{85A196E6-04A4-435C-9244-08FABA40BC61}" name="AF_1" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
       <totalsRowFormula>SUM(D6:D29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{65FF0D36-7E63-4320-A7F3-263DC9CE365C}" name="AF_2" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="7">
+    <tableColumn id="5" xr3:uid="{65FF0D36-7E63-4320-A7F3-263DC9CE365C}" name="AF_2" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
       <totalsRowFormula>SUM(E6:E29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{53F01DBB-865D-4EB2-B7AE-ECDC942AB144}" name="CAN_1" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="6">
+    <tableColumn id="6" xr3:uid="{53F01DBB-865D-4EB2-B7AE-ECDC942AB144}" name="CAN_1" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUM(F6:F29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{CB89D53A-340F-4C1B-BCBD-B920A9A91BC2}" name="CAN_2" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="5">
+    <tableColumn id="7" xr3:uid="{CB89D53A-340F-4C1B-BCBD-B920A9A91BC2}" name="CAN_2" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUM(G6:G29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{1BB3BCD2-3465-4992-B900-2686199AC0B2}" name="BC_1" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="4">
+    <tableColumn id="8" xr3:uid="{1BB3BCD2-3465-4992-B900-2686199AC0B2}" name="BC_1" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
       <totalsRowFormula>SUM(H6:H29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C1DFD320-902F-4A24-9D80-A14DA5525354}" name="BC_2" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="3">
+    <tableColumn id="9" xr3:uid="{C1DFD320-902F-4A24-9D80-A14DA5525354}" name="BC_2" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUM(I6:I29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7D4C682B-C904-4BB5-B41A-CFFF148C5415}" name="Season Average" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="11">
+    <tableColumn id="11" xr3:uid="{7D4C682B-C904-4BB5-B41A-CFFF148C5415}" name="Season Average" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</calculatedColumnFormula>
       <totalsRowFormula>SUM(J6:J29)</totalsRowFormula>
     </tableColumn>
@@ -2938,7 +2929,7 @@
     <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:J26">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="7">
@@ -2976,8 +2967,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2995,864 +2986,856 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
+      <c r="A2" s="22"/>
     </row>
     <row r="3" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="18"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="18"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="29" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>2.125</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>1.4007932692307601</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>2.0099999999999998</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>0.75</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>1.77079326923076</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>0.39579326923076902</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>1.825</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>0.33999999999999903</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.327172475961536</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>0.67499999999999905</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>1.1849999999999901</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>1.28</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>1.1949999999999901</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>1.21</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>1.07079326923076</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>2.2207932692307599</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <v>1.31079326923076</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.2684224759615326</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>2.2799999999999998</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>1.5249999999999999</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>1.4407932692307599</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>0.31</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>0.72579326923076903</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>1.84</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>1.0149999999999999</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>0.47</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.2008233173076912</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>0.995</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>1.16499999999999</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>0.86499999999999999</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>3.03</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>1.2749999999999999</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <v>0.61</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>0.92999999999999905</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>0.36499999999999999</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.1543749999999986</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>1.6707932692307601</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>0.149999999999999</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>1.0149999999999999</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>0.63999999999999901</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>1.7949999999999999</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <v>0.93</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>1.335</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>1.17579326923076</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.0889483173076897</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>0.52499999999999902</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>1.0149999999999999</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>1.125</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>0.50079326923076894</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>2.7749999999999999</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <v>1.2207932692307599</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>0.32079326923076901</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>0.32079326923076901</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.9753966346153834</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>0.92079326923076898</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>1.905</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>0.45</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>0.51079326923076895</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>0.97499999999999998</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <v>1.61499999999999</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>0.54579326923076898</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>0.71499999999999997</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.95467247596153704</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>0.67499999999999905</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>1.2749999999999999</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>1.53079326923076</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>-0.22499999999999901</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <v>1.9549999999999901</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <v>0.6</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>1.165</v>
       </c>
-      <c r="I13" s="11">
-        <v>0</v>
-      </c>
-      <c r="J13" s="20">
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.87197415865384365</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>1.155</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>0.29999999999999899</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <v>1.425</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>0.75</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <v>1.24</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="10">
         <v>0.22499999999999901</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <v>1.165</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="10">
         <v>0.375</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.82937499999999975</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>2.0649999999999902</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>0.149999999999999</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <v>0.67500000000000004</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>0.33</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="10">
         <v>0.85499999999999998</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="10">
         <v>1.155</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>0.85499999999999998</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="10">
         <v>0.22499999999999901</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.7887499999999984</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>1.23999999999999</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>0.86499999999999999</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>1.165</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>0.17079326923076901</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <v>0.62079326923076905</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <v>0.49158653846153799</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>1.2</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>0.23499999999999999</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.74852163461538335</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>0.82079326923076901</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>0.875</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <v>0.73579326923076904</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>-0.29499999999999998</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <v>1.1323798076923</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="10">
         <v>1.99999999999999E-2</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="10">
         <v>0.51579326923076896</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="10">
         <v>0.53500000000000003</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.5424699519230759</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>1.0049999999999999</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>0.62079326923076905</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <v>0.69579326923076901</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>-0.15</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <v>0.15</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="10">
         <v>0.49158653846153799</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>1.0373798076923</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="10">
         <v>0.44999999999999901</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.53756911057692192</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <v>0.374999999999999</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <v>0.22499999999999901</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="10">
         <v>1.7849999999999999</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>-5.4206730769230702E-2</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <v>1.165</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="10">
         <v>0.15</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="10">
         <v>0.375</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="10">
         <v>0.22499999999999901</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.5307241586538457</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>0.6</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>0.149999999999999</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="10">
         <v>0.69579326923076901</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <v>-7.4999999999999997E-2</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="10">
         <v>1.2749999999999999</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="10">
         <v>0.86499999999999999</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="10">
         <v>0.3</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="10">
         <v>0.375</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.52322415865384597</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <v>1.3149999999999999</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>0.44999999999999901</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="10">
         <v>0.52500000000000002</v>
       </c>
-      <c r="E21" s="11">
-        <v>0</v>
-      </c>
-      <c r="F21" s="11">
+      <c r="E21" s="10">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10">
         <v>0.52499999999999902</v>
       </c>
-      <c r="G21" s="11">
-        <v>0</v>
-      </c>
-      <c r="H21" s="11">
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="H21" s="10">
         <v>0.44999999999999901</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="10">
         <v>0.39579326923076902</v>
       </c>
-      <c r="J21" s="20">
+      <c r="J21" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.45759915865384576</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <v>1.165</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="10">
         <v>0.23499999999999899</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="10">
         <v>0.77079326923076896</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="10">
         <v>-0.22499999999999901</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <v>0.3</v>
       </c>
-      <c r="G22" s="11">
-        <v>0</v>
-      </c>
-      <c r="H22" s="11">
+      <c r="G22" s="10">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
         <v>0.375</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="10">
         <v>0.15</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.34634915865384613</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11">
-        <v>0</v>
-      </c>
-      <c r="C23" s="11">
-        <v>0</v>
-      </c>
-      <c r="D23" s="11">
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
         <v>1.24</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="10">
         <v>-0.375</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <v>0.54579326923076898</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="10">
         <v>7.49999999999999E-2</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="10">
         <v>0.69579326923076901</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="10">
         <v>0.15</v>
       </c>
-      <c r="J23" s="20">
+      <c r="J23" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.29144831730769222</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="10">
         <v>1.5</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="10">
         <v>7.49999999999999E-2</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="10">
         <v>0.62079326923076905</v>
       </c>
-      <c r="E24" s="11">
-        <v>0</v>
-      </c>
-      <c r="F24" s="11">
-        <v>0</v>
-      </c>
-      <c r="G24" s="11">
-        <v>0</v>
-      </c>
-      <c r="H24" s="11">
-        <v>0</v>
-      </c>
-      <c r="I24" s="11">
-        <v>0</v>
-      </c>
-      <c r="J24" s="20">
+      <c r="E24" s="10">
+        <v>0</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
+      <c r="G24" s="10">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0</v>
+      </c>
+      <c r="I24" s="10">
+        <v>0</v>
+      </c>
+      <c r="J24" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.27447415865384611</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <v>0.44999999999999901</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <v>1.3357932692307599</v>
       </c>
-      <c r="D25" s="11">
-        <v>0</v>
-      </c>
-      <c r="E25" s="11">
-        <v>0</v>
-      </c>
-      <c r="F25" s="11">
-        <v>0</v>
-      </c>
-      <c r="G25" s="11">
-        <v>0</v>
-      </c>
-      <c r="H25" s="11">
-        <v>0</v>
-      </c>
-      <c r="I25" s="11">
-        <v>0</v>
-      </c>
-      <c r="J25" s="20">
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="10">
+        <v>0</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0</v>
+      </c>
+      <c r="I25" s="10">
+        <v>0</v>
+      </c>
+      <c r="J25" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.22322415865384487</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="11">
-        <v>0</v>
-      </c>
-      <c r="C26" s="11">
-        <v>0</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0</v>
-      </c>
-      <c r="E26" s="11">
+      <c r="B26" s="10">
+        <v>0</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10">
         <v>-0.22499999999999901</v>
       </c>
-      <c r="F26" s="11">
-        <v>0</v>
-      </c>
-      <c r="G26" s="11">
+      <c r="F26" s="10">
+        <v>0</v>
+      </c>
+      <c r="G26" s="10">
         <v>0.49158653846153799</v>
       </c>
-      <c r="H26" s="11">
-        <v>0</v>
-      </c>
-      <c r="I26" s="11">
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10">
         <v>0.3</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>7.0823317307692368E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="11">
-        <v>0</v>
-      </c>
-      <c r="C27" s="11">
-        <v>0</v>
-      </c>
-      <c r="D27" s="11">
-        <v>0</v>
-      </c>
-      <c r="E27" s="11">
-        <v>0</v>
-      </c>
-      <c r="F27" s="11">
+      <c r="B27" s="10">
+        <v>0</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0</v>
+      </c>
+      <c r="F27" s="10">
         <v>0.22499999999999901</v>
       </c>
-      <c r="G27" s="11">
-        <v>0</v>
-      </c>
-      <c r="H27" s="11">
-        <v>0</v>
-      </c>
-      <c r="I27" s="11">
-        <v>0</v>
-      </c>
-      <c r="J27" s="20">
+      <c r="G27" s="10">
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10">
+        <v>0</v>
+      </c>
+      <c r="J27" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>2.8124999999999876E-2</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="11">
-        <v>0</v>
-      </c>
-      <c r="C28" s="11">
-        <v>0</v>
-      </c>
-      <c r="D28" s="11">
-        <v>0</v>
-      </c>
-      <c r="E28" s="11">
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
         <v>-0.3</v>
       </c>
-      <c r="F28" s="11">
-        <v>0</v>
-      </c>
-      <c r="G28" s="11">
-        <v>0</v>
-      </c>
-      <c r="H28" s="11">
-        <v>0</v>
-      </c>
-      <c r="I28" s="11">
+      <c r="F28" s="10">
+        <v>0</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10">
         <v>0.29999999999999899</v>
       </c>
-      <c r="J28" s="20">
+      <c r="J28" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>-1.2490009027033011E-16</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="12">
-        <v>0</v>
-      </c>
-      <c r="C29" s="12">
-        <v>0</v>
-      </c>
-      <c r="D29" s="12">
-        <v>0</v>
-      </c>
-      <c r="E29" s="12">
-        <v>0</v>
-      </c>
-      <c r="F29" s="12">
-        <v>0</v>
-      </c>
-      <c r="G29" s="12">
+      <c r="B29" s="11">
+        <v>0</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11">
+        <v>0</v>
+      </c>
+      <c r="G29" s="11">
         <v>-7.4999999999999997E-2</v>
       </c>
-      <c r="H29" s="12">
-        <v>0</v>
-      </c>
-      <c r="I29" s="12">
-        <v>0</v>
-      </c>
-      <c r="J29" s="20">
+      <c r="H29" s="11">
+        <v>0</v>
+      </c>
+      <c r="I29" s="11">
+        <v>0</v>
+      </c>
+      <c r="J29" s="18">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>-9.3749999999999997E-3</v>
       </c>
@@ -3870,43 +3853,43 @@
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="21">
-        <f>SUM(B6:B29)</f>
+      <c r="B31" s="19">
+        <f t="shared" ref="B31:J31" si="0">SUM(B6:B29)</f>
         <v>21.557379807692275</v>
       </c>
-      <c r="C31" s="21">
-        <f>SUM(C6:C29)</f>
+      <c r="C31" s="19">
+        <f t="shared" si="0"/>
         <v>14.902379807692261</v>
       </c>
-      <c r="D31" s="21">
-        <f>SUM(D6:D29)</f>
+      <c r="D31" s="19">
+        <f t="shared" si="0"/>
         <v>20.050552884615364</v>
       </c>
-      <c r="E31" s="21">
-        <f>SUM(E6:E29)</f>
+      <c r="E31" s="19">
+        <f t="shared" si="0"/>
         <v>6.263173076923068</v>
       </c>
-      <c r="F31" s="21">
-        <f>SUM(F6:F29)</f>
+      <c r="F31" s="19">
+        <f t="shared" si="0"/>
         <v>20.515552884615349</v>
       </c>
-      <c r="G31" s="21">
-        <f>SUM(G6:G29)</f>
+      <c r="G31" s="19">
+        <f t="shared" si="0"/>
         <v>12.172139423076892</v>
       </c>
-      <c r="H31" s="21">
-        <f>SUM(H6:H29)</f>
+      <c r="H31" s="19">
+        <f t="shared" si="0"/>
         <v>16.326346153846135</v>
       </c>
-      <c r="I31" s="21">
-        <f>SUM(I6:I29)</f>
+      <c r="I31" s="19">
+        <f t="shared" si="0"/>
         <v>8.4131730769230533</v>
       </c>
-      <c r="J31" s="13">
-        <f>SUM(J6:J29)</f>
+      <c r="J31" s="12">
+        <f t="shared" si="0"/>
         <v>15.025087139423047</v>
       </c>
     </row>
@@ -3926,30 +3909,30 @@
       <c r="J33" s="28"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
     </row>
     <row r="35" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30" t="s">
+      <c r="A35" s="24"/>
+      <c r="B35" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
before I break something. see you monday
</commit_message>
<xml_diff>
--- a/data/MANUAL_Nov_2_MSU_GAME_SCORES.xlsx
+++ b/data/MANUAL_Nov_2_MSU_GAME_SCORES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\college_hockey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5289F748-D915-47D7-A209-EF70A4DF6FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13062ED2-DFAE-42EB-B8BF-76C5D2A08184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-16050" yWindow="4545" windowWidth="18900" windowHeight="11505" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nov_2_MSU_GAME_SCORES" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Player</t>
   </si>
@@ -159,6 +159,9 @@
                                   + FACEOFFS [ (FOW * 0.01) - ( FOL *0.01) ]
                                   + TEAM [ EVEN STRENGTH (Goals For *0.15) + (Goals Against *0.15) ]
                                   - PENALTY  [ (Penalties * PP Success Rate) ]  </t>
+  </si>
+  <si>
+    <t>Season Total</t>
   </si>
 </sst>
 </file>
@@ -818,25 +821,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -876,9 +869,28 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -924,51 +936,30 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="30">
     <dxf>
       <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color theme="0"/>
+        <color theme="1"/>
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -990,45 +981,16 @@
           <bgColor rgb="FF18453B"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1042,7 +1004,8 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -1051,34 +1014,7 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1092,7 +1028,8 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -1101,34 +1038,7 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1142,7 +1052,8 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -1151,34 +1062,7 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1192,7 +1076,8 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -1201,34 +1086,7 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1242,7 +1100,8 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -1251,34 +1110,7 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1292,7 +1124,8 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -1301,34 +1134,7 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1342,43 +1148,7 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Roboto Slab"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF18453B"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1409,11 +1179,281 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="164" formatCode="0.000"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Roboto Slab"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF18453B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1429,6 +1469,38 @@
         <name val="Roboto Slab"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1516,15 +1588,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>171038</xdr:colOff>
+      <xdr:colOff>56738</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>577195</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>34270</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>581025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1553,7 +1625,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3314288" y="571500"/>
+          <a:off x="3142838" y="247650"/>
           <a:ext cx="1025282" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1566,15 +1638,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>352425</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>561975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1603,7 +1675,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2066925" y="542925"/>
+          <a:off x="2009775" y="200025"/>
           <a:ext cx="1057275" cy="1057275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1616,15 +1688,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>257176</xdr:colOff>
+      <xdr:colOff>123826</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>389279</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>332129</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>561975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1653,7 +1725,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4638676" y="571500"/>
+          <a:off x="4257676" y="247650"/>
           <a:ext cx="751228" cy="1009650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1665,16 +1737,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>428625</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>567718</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>62893</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>523875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1703,7 +1775,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5724525" y="619125"/>
+          <a:off x="5162550" y="238125"/>
           <a:ext cx="1082068" cy="981075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1732,7 +1804,7 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="CAN_2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="BC_1"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BC_2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="SEASON_AVG" dataDxfId="25">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="SEASON_AVG" dataDxfId="29">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[LSSU_1]:[BC_2]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1741,8 +1813,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD3ED04E-82AE-4CFB-A8EC-BB33F4837DB9}" name="Table14" displayName="Table14" ref="A5:J31" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22">
-  <autoFilter ref="A5:J30" xr:uid="{FD3ED04E-82AE-4CFB-A8EC-BB33F4837DB9}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FD3ED04E-82AE-4CFB-A8EC-BB33F4837DB9}" name="Table14" displayName="Table14" ref="A5:K31" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
+  <autoFilter ref="A5:K30" xr:uid="{FD3ED04E-82AE-4CFB-A8EC-BB33F4837DB9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1753,39 +1825,43 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
     <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J29">
     <sortCondition descending="1" ref="J5:J29"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{92A4CFC6-961E-4C81-A091-04B59744BA36}" name="Player" totalsRowLabel="TOTAL" dataDxfId="21" totalsRowDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{018653C9-4BD5-4955-BD88-FF0901ED735D}" name="LSSU_1" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{92A4CFC6-961E-4C81-A091-04B59744BA36}" name="Player" totalsRowLabel="TOTAL" dataDxfId="9" totalsRowDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{018653C9-4BD5-4955-BD88-FF0901ED735D}" name="LSSU_1" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="19">
       <totalsRowFormula>SUM(B6:B29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8AA04EE0-25FB-4161-8387-A764CBF8C414}" name="LSSU_2" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
+    <tableColumn id="3" xr3:uid="{8AA04EE0-25FB-4161-8387-A764CBF8C414}" name="LSSU_2" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="18">
       <totalsRowFormula>SUM(C6:C29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{85A196E6-04A4-435C-9244-08FABA40BC61}" name="AF_1" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="4" xr3:uid="{85A196E6-04A4-435C-9244-08FABA40BC61}" name="AF_1" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="17">
       <totalsRowFormula>SUM(D6:D29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{65FF0D36-7E63-4320-A7F3-263DC9CE365C}" name="AF_2" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="5" xr3:uid="{65FF0D36-7E63-4320-A7F3-263DC9CE365C}" name="AF_2" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="16">
       <totalsRowFormula>SUM(E6:E29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{53F01DBB-865D-4EB2-B7AE-ECDC942AB144}" name="CAN_1" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="6" xr3:uid="{53F01DBB-865D-4EB2-B7AE-ECDC942AB144}" name="CAN_1" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="15">
       <totalsRowFormula>SUM(F6:F29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{CB89D53A-340F-4C1B-BCBD-B920A9A91BC2}" name="CAN_2" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="7" xr3:uid="{CB89D53A-340F-4C1B-BCBD-B920A9A91BC2}" name="CAN_2" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="14">
       <totalsRowFormula>SUM(G6:G29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{1BB3BCD2-3465-4992-B900-2686199AC0B2}" name="BC_1" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="8" xr3:uid="{1BB3BCD2-3465-4992-B900-2686199AC0B2}" name="BC_1" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="13">
       <totalsRowFormula>SUM(H6:H29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C1DFD320-902F-4A24-9D80-A14DA5525354}" name="BC_2" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="9" xr3:uid="{C1DFD320-902F-4A24-9D80-A14DA5525354}" name="BC_2" totalsRowFunction="custom" dataDxfId="0" totalsRowDxfId="12">
       <totalsRowFormula>SUM(I6:I29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7D4C682B-C904-4BB5-B41A-CFFF148C5415}" name="Season Average" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="11" xr3:uid="{7D4C682B-C904-4BB5-B41A-CFFF148C5415}" name="Season Average" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="11">
       <calculatedColumnFormula>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</calculatedColumnFormula>
       <totalsRowFormula>SUM(J6:J29)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{85902DB4-3403-43AF-A813-C0837DB1BA43}" name="Season Total" dataDxfId="23" totalsRowDxfId="10">
+      <calculatedColumnFormula>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -2929,7 +3005,7 @@
     <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:J26">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="7">
@@ -2965,974 +3041,1084 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-    </row>
-    <row r="3" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="20" t="s">
+    <row r="2" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="18"/>
+    </row>
+    <row r="3" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="17" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="13" t="s">
+      <c r="K5" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="29">
         <v>2.125</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="29">
         <v>1.4007932692307601</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="29">
         <v>2.0099999999999998</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="29">
         <v>0.75</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="29">
         <v>1.77079326923076</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="29">
         <v>0.39579326923076902</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="29">
         <v>1.825</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="29">
         <v>0.33999999999999903</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.327172475961536</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="14" t="s">
+      <c r="K6" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>10.617379807692288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="30">
         <v>0.67499999999999905</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="30">
         <v>1.1849999999999901</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="30">
         <v>1.28</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="30">
         <v>1.1949999999999901</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="30">
         <v>1.21</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="30">
         <v>1.07079326923076</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="30">
         <v>2.2207932692307599</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="30">
         <v>1.31079326923076</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.2684224759615326</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A8" s="14" t="s">
+      <c r="K7" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>10.147379807692261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="30">
         <v>2.2799999999999998</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="30">
         <v>1.5249999999999999</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="30">
         <v>1.4407932692307599</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="30">
         <v>0.31</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="30">
         <v>0.72579326923076903</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="30">
         <v>1.84</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="30">
         <v>1.0149999999999999</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="30">
         <v>0.47</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.2008233173076912</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="14" t="s">
+      <c r="K8" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>9.6065865384615297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="30">
         <v>0.995</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="30">
         <v>1.16499999999999</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="30">
         <v>0.86499999999999999</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="30">
         <v>3.03</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="30">
         <v>1.2749999999999999</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="30">
         <v>0.61</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="30">
         <v>0.92999999999999905</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="30">
         <v>0.36499999999999999</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.1543749999999986</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A10" s="14" t="s">
+      <c r="K9" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>9.2349999999999888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="30">
         <v>1.6707932692307601</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="30">
         <v>0.149999999999999</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="30">
         <v>1.0149999999999999</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="30">
         <v>0.63999999999999901</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="30">
         <v>1.7949999999999999</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="30">
         <v>0.93</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="30">
         <v>1.335</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="30">
         <v>1.17579326923076</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>1.0889483173076897</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="14" t="s">
+      <c r="K10" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>8.7115865384615176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="30">
         <v>0.52499999999999902</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="30">
         <v>1.0149999999999999</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="30">
         <v>1.125</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="30">
         <v>0.50079326923076894</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="30">
         <v>2.7749999999999999</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="30">
         <v>1.2207932692307599</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="30">
         <v>0.32079326923076901</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="30">
         <v>0.32079326923076901</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.9753966346153834</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="14" t="s">
+      <c r="K11" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>7.8031730769230672</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="30">
         <v>0.92079326923076898</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="30">
         <v>1.905</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="30">
         <v>0.45</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="30">
         <v>0.51079326923076895</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="30">
         <v>0.97499999999999998</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="30">
         <v>1.61499999999999</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="30">
         <v>0.54579326923076898</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="30">
         <v>0.71499999999999997</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.95467247596153704</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
+      <c r="K12" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>7.6373798076922963</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="30">
         <v>0.67499999999999905</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="30">
         <v>1.2749999999999999</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="30">
         <v>1.53079326923076</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="30">
         <v>-0.22499999999999901</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="30">
         <v>1.9549999999999901</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="30">
         <v>0.6</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="30">
         <v>1.165</v>
       </c>
-      <c r="I13" s="10">
-        <v>0</v>
-      </c>
-      <c r="J13" s="18">
+      <c r="I13" s="30">
+        <v>0</v>
+      </c>
+      <c r="J13" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.87197415865384365</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="14" t="s">
+      <c r="K13" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>6.9757932692307492</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="30">
         <v>1.155</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="30">
         <v>0.29999999999999899</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="30">
         <v>1.425</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="30">
         <v>0.75</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="30">
         <v>1.24</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="30">
         <v>0.22499999999999901</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="30">
         <v>1.165</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="30">
         <v>0.375</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.82937499999999975</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="14" t="s">
+      <c r="K14" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>6.634999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="30">
         <v>2.0649999999999902</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="30">
         <v>0.149999999999999</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="30">
         <v>0.67500000000000004</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="30">
         <v>0.33</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="30">
         <v>0.85499999999999998</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="30">
         <v>1.155</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="30">
         <v>0.85499999999999998</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="30">
         <v>0.22499999999999901</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.7887499999999984</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="14" t="s">
+      <c r="K15" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>6.3099999999999872</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A16" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="30">
         <v>1.23999999999999</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="30">
         <v>0.86499999999999999</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="30">
         <v>1.165</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="30">
         <v>0.17079326923076901</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="30">
         <v>0.62079326923076905</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="30">
         <v>0.49158653846153799</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="30">
         <v>1.2</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="30">
         <v>0.23499999999999999</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.74852163461538335</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A17" s="14" t="s">
+      <c r="K16" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>5.9881730769230668</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="30">
         <v>0.82079326923076901</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="30">
         <v>0.875</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="30">
         <v>0.73579326923076904</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="30">
         <v>-0.29499999999999998</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="30">
         <v>1.1323798076923</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="30">
         <v>1.99999999999999E-2</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="30">
         <v>0.51579326923076896</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="30">
         <v>0.53500000000000003</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.5424699519230759</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A18" s="14" t="s">
+      <c r="K17" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>4.3397596153846072</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="30">
         <v>1.0049999999999999</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="30">
         <v>0.62079326923076905</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="30">
         <v>0.69579326923076901</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="30">
         <v>-0.15</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="30">
         <v>0.15</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="30">
         <v>0.49158653846153799</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="30">
         <v>1.0373798076923</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="30">
         <v>0.44999999999999901</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.53756911057692192</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A19" s="14" t="s">
+      <c r="K18" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>4.3005528846153753</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="30">
         <v>0.374999999999999</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="30">
         <v>0.22499999999999901</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="30">
         <v>1.7849999999999999</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="30">
         <v>-5.4206730769230702E-2</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="30">
         <v>1.165</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="30">
         <v>0.15</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="30">
         <v>0.375</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="30">
         <v>0.22499999999999901</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.5307241586538457</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A20" s="14" t="s">
+      <c r="K19" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>4.2457932692307656</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="30">
         <v>0.6</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="30">
         <v>0.149999999999999</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="30">
         <v>0.69579326923076901</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="30">
         <v>-7.4999999999999997E-2</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="30">
         <v>1.2749999999999999</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="30">
         <v>0.86499999999999999</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="30">
         <v>0.3</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="30">
         <v>0.375</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.52322415865384597</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A21" s="14" t="s">
+      <c r="K20" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>4.1857932692307678</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="30">
         <v>1.3149999999999999</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="30">
         <v>0.44999999999999901</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="30">
         <v>0.52500000000000002</v>
       </c>
-      <c r="E21" s="10">
-        <v>0</v>
-      </c>
-      <c r="F21" s="10">
+      <c r="E21" s="30">
+        <v>0</v>
+      </c>
+      <c r="F21" s="30">
         <v>0.52499999999999902</v>
       </c>
-      <c r="G21" s="10">
-        <v>0</v>
-      </c>
-      <c r="H21" s="10">
+      <c r="G21" s="30">
+        <v>0</v>
+      </c>
+      <c r="H21" s="30">
         <v>0.44999999999999901</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="30">
         <v>0.39579326923076902</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J21" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.45759915865384576</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A22" s="14" t="s">
+      <c r="K21" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>3.6607932692307661</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="30">
         <v>1.165</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="30">
         <v>0.23499999999999899</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="30">
         <v>0.77079326923076896</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="30">
         <v>-0.22499999999999901</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="30">
         <v>0.3</v>
       </c>
-      <c r="G22" s="10">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10">
+      <c r="G22" s="30">
+        <v>0</v>
+      </c>
+      <c r="H22" s="30">
         <v>0.375</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="30">
         <v>0.15</v>
       </c>
-      <c r="J22" s="18">
+      <c r="J22" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.34634915865384613</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A23" s="14" t="s">
+      <c r="K22" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>2.7707932692307691</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A23" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="10">
-        <v>0</v>
-      </c>
-      <c r="C23" s="10">
-        <v>0</v>
-      </c>
-      <c r="D23" s="10">
+      <c r="B23" s="30">
+        <v>0</v>
+      </c>
+      <c r="C23" s="30">
+        <v>0</v>
+      </c>
+      <c r="D23" s="30">
         <v>1.24</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="30">
         <v>-0.375</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="30">
         <v>0.54579326923076898</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="30">
         <v>7.49999999999999E-2</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="30">
         <v>0.69579326923076901</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="30">
         <v>0.15</v>
       </c>
-      <c r="J23" s="18">
+      <c r="J23" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.29144831730769222</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A24" s="14" t="s">
+      <c r="K23" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>2.3315865384615377</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="30">
         <v>1.5</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="30">
         <v>7.49999999999999E-2</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="30">
         <v>0.62079326923076905</v>
       </c>
-      <c r="E24" s="10">
-        <v>0</v>
-      </c>
-      <c r="F24" s="10">
-        <v>0</v>
-      </c>
-      <c r="G24" s="10">
-        <v>0</v>
-      </c>
-      <c r="H24" s="10">
-        <v>0</v>
-      </c>
-      <c r="I24" s="10">
-        <v>0</v>
-      </c>
-      <c r="J24" s="18">
+      <c r="E24" s="30">
+        <v>0</v>
+      </c>
+      <c r="F24" s="30">
+        <v>0</v>
+      </c>
+      <c r="G24" s="30">
+        <v>0</v>
+      </c>
+      <c r="H24" s="30">
+        <v>0</v>
+      </c>
+      <c r="I24" s="30">
+        <v>0</v>
+      </c>
+      <c r="J24" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.27447415865384611</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A25" s="14" t="s">
+      <c r="K24" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>2.1957932692307689</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="30">
         <v>0.44999999999999901</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="30">
         <v>1.3357932692307599</v>
       </c>
-      <c r="D25" s="10">
-        <v>0</v>
-      </c>
-      <c r="E25" s="10">
-        <v>0</v>
-      </c>
-      <c r="F25" s="10">
-        <v>0</v>
-      </c>
-      <c r="G25" s="10">
-        <v>0</v>
-      </c>
-      <c r="H25" s="10">
-        <v>0</v>
-      </c>
-      <c r="I25" s="10">
-        <v>0</v>
-      </c>
-      <c r="J25" s="18">
+      <c r="D25" s="30">
+        <v>0</v>
+      </c>
+      <c r="E25" s="30">
+        <v>0</v>
+      </c>
+      <c r="F25" s="30">
+        <v>0</v>
+      </c>
+      <c r="G25" s="30">
+        <v>0</v>
+      </c>
+      <c r="H25" s="30">
+        <v>0</v>
+      </c>
+      <c r="I25" s="30">
+        <v>0</v>
+      </c>
+      <c r="J25" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>0.22322415865384487</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="14" t="s">
+      <c r="K25" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>1.785793269230759</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A26" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="10">
-        <v>0</v>
-      </c>
-      <c r="C26" s="10">
-        <v>0</v>
-      </c>
-      <c r="D26" s="10">
-        <v>0</v>
-      </c>
-      <c r="E26" s="10">
+      <c r="B26" s="30">
+        <v>0</v>
+      </c>
+      <c r="C26" s="30">
+        <v>0</v>
+      </c>
+      <c r="D26" s="30">
+        <v>0</v>
+      </c>
+      <c r="E26" s="30">
         <v>-0.22499999999999901</v>
       </c>
-      <c r="F26" s="10">
-        <v>0</v>
-      </c>
-      <c r="G26" s="10">
+      <c r="F26" s="30">
+        <v>0</v>
+      </c>
+      <c r="G26" s="30">
         <v>0.49158653846153799</v>
       </c>
-      <c r="H26" s="10">
-        <v>0</v>
-      </c>
-      <c r="I26" s="10">
+      <c r="H26" s="30">
+        <v>0</v>
+      </c>
+      <c r="I26" s="30">
         <v>0.3</v>
       </c>
-      <c r="J26" s="18">
+      <c r="J26" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>7.0823317307692368E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="14" t="s">
+      <c r="K26" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>0.56658653846153895</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A27" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="10">
-        <v>0</v>
-      </c>
-      <c r="C27" s="10">
-        <v>0</v>
-      </c>
-      <c r="D27" s="10">
-        <v>0</v>
-      </c>
-      <c r="E27" s="10">
-        <v>0</v>
-      </c>
-      <c r="F27" s="10">
+      <c r="B27" s="30">
+        <v>0</v>
+      </c>
+      <c r="C27" s="30">
+        <v>0</v>
+      </c>
+      <c r="D27" s="30">
+        <v>0</v>
+      </c>
+      <c r="E27" s="30">
+        <v>0</v>
+      </c>
+      <c r="F27" s="30">
         <v>0.22499999999999901</v>
       </c>
-      <c r="G27" s="10">
-        <v>0</v>
-      </c>
-      <c r="H27" s="10">
-        <v>0</v>
-      </c>
-      <c r="I27" s="10">
-        <v>0</v>
-      </c>
-      <c r="J27" s="18">
+      <c r="G27" s="30">
+        <v>0</v>
+      </c>
+      <c r="H27" s="30">
+        <v>0</v>
+      </c>
+      <c r="I27" s="30">
+        <v>0</v>
+      </c>
+      <c r="J27" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>2.8124999999999876E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="14" t="s">
+      <c r="K27" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>0.22499999999999901</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A28" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="10">
-        <v>0</v>
-      </c>
-      <c r="C28" s="10">
-        <v>0</v>
-      </c>
-      <c r="D28" s="10">
-        <v>0</v>
-      </c>
-      <c r="E28" s="10">
+      <c r="B28" s="30">
+        <v>0</v>
+      </c>
+      <c r="C28" s="30">
+        <v>0</v>
+      </c>
+      <c r="D28" s="30">
+        <v>0</v>
+      </c>
+      <c r="E28" s="30">
         <v>-0.3</v>
       </c>
-      <c r="F28" s="10">
-        <v>0</v>
-      </c>
-      <c r="G28" s="10">
-        <v>0</v>
-      </c>
-      <c r="H28" s="10">
-        <v>0</v>
-      </c>
-      <c r="I28" s="10">
+      <c r="F28" s="30">
+        <v>0</v>
+      </c>
+      <c r="G28" s="30">
+        <v>0</v>
+      </c>
+      <c r="H28" s="30">
+        <v>0</v>
+      </c>
+      <c r="I28" s="30">
         <v>0.29999999999999899</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>-1.2490009027033011E-16</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="15" t="s">
+      <c r="K28" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>-9.9920072216264089E-16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="11">
-        <v>0</v>
-      </c>
-      <c r="C29" s="11">
-        <v>0</v>
-      </c>
-      <c r="D29" s="11">
-        <v>0</v>
-      </c>
-      <c r="E29" s="11">
-        <v>0</v>
-      </c>
-      <c r="F29" s="11">
-        <v>0</v>
-      </c>
-      <c r="G29" s="11">
+      <c r="B29" s="31">
+        <v>0</v>
+      </c>
+      <c r="C29" s="31">
+        <v>0</v>
+      </c>
+      <c r="D29" s="31">
+        <v>0</v>
+      </c>
+      <c r="E29" s="31">
+        <v>0</v>
+      </c>
+      <c r="F29" s="31">
+        <v>0</v>
+      </c>
+      <c r="G29" s="31">
         <v>-7.4999999999999997E-2</v>
       </c>
-      <c r="H29" s="11">
-        <v>0</v>
-      </c>
-      <c r="I29" s="11">
-        <v>0</v>
-      </c>
-      <c r="J29" s="18">
+      <c r="H29" s="31">
+        <v>0</v>
+      </c>
+      <c r="I29" s="31">
+        <v>0</v>
+      </c>
+      <c r="J29" s="14">
         <f>AVERAGE(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
         <v>-9.3749999999999997E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" ht="21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="K29" s="14">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>-7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="3" customFormat="1" ht="21" hidden="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A31" s="8" t="s">
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="26">
+        <f>SUM(Table14[[#This Row],[LSSU_1]:[BC_2]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="15">
         <f t="shared" ref="B31:J31" si="0">SUM(B6:B29)</f>
         <v>21.557379807692275</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="15">
         <f t="shared" si="0"/>
         <v>14.902379807692261</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="15">
         <f t="shared" si="0"/>
         <v>20.050552884615364</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="15">
         <f t="shared" si="0"/>
         <v>6.263173076923068</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="15">
         <f t="shared" si="0"/>
         <v>20.515552884615349</v>
       </c>
-      <c r="G31" s="19">
+      <c r="G31" s="15">
         <f t="shared" si="0"/>
         <v>12.172139423076892</v>
       </c>
-      <c r="H31" s="19">
+      <c r="H31" s="15">
         <f t="shared" si="0"/>
         <v>16.326346153846135</v>
       </c>
-      <c r="I31" s="19">
+      <c r="I31" s="15">
         <f t="shared" si="0"/>
         <v>8.4131730769230533</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="8">
         <f t="shared" si="0"/>
         <v>15.025087139423047</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="K31" s="15"/>
+    </row>
+    <row r="32" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
     </row>
     <row r="35" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24"/>
-      <c r="B35" s="26" t="s">
+      <c r="A35" s="20"/>
+      <c r="B35" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3945,7 +4131,32 @@
     <mergeCell ref="A33:J33"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:J30">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:J29">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="40"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6:K29">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -3957,7 +4168,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:J29">
+  <conditionalFormatting sqref="K6:K29">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>